<commit_message>
arreglar campos de producto y categoria
arreglar campos de producto y categoria
</commit_message>
<xml_diff>
--- a/CompuOfertas/SIGPAdProject/SIGPAd/static/documents/exampleCategoria.xlsx
+++ b/CompuOfertas/SIGPAdProject/SIGPAd/static/documents/exampleCategoria.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Computadoras</t>
   </si>
   <si>
     <t>todo lo relacionado a las computadoras de escritorio</t>
-  </si>
-  <si>
-    <t>nose para que es esto</t>
   </si>
   <si>
     <t>Laptop</t>
@@ -394,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,9 +405,9 @@
     <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -418,50 +415,38 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>